<commit_message>
CP terminados, actualizado el script de precondiciones
</commit_message>
<xml_diff>
--- a/Producto/Web/Casos de prueba/10.xlsx
+++ b/Producto/Web/Casos de prueba/10.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
   <si>
     <t>ID</t>
   </si>
@@ -91,10 +91,25 @@
     <t>Registrar un usuario en la base de datos</t>
   </si>
   <si>
-    <t>El usuario "CPA_Usuario" no existe en la base de datos</t>
-  </si>
-  <si>
     <t>ingreso al sistema.</t>
+  </si>
+  <si>
+    <t>Selecciono la opcion Ingresar</t>
+  </si>
+  <si>
+    <t>El sistema muestra un popup para iniciar sesion o registrarse.</t>
+  </si>
+  <si>
+    <t>El usuario "CPA_Usuario" existe en la base de datos</t>
+  </si>
+  <si>
+    <t>Ingreso "CPA_Usuario" en el campo usuario y "CPA_Contraseña" en el campo contraseña</t>
+  </si>
+  <si>
+    <t>Seleccióno la opcion Iniciar sesion</t>
+  </si>
+  <si>
+    <t>El sistema muestra el nombre de usuario donde antes estaba la opcion Ingresar</t>
   </si>
 </sst>
 </file>
@@ -574,7 +589,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -654,7 +669,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -674,12 +689,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="25.5">
+    <row r="2" spans="1:3">
       <c r="A2" s="7">
         <v>1</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -695,7 +710,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -724,33 +739,43 @@
         <v>1</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:4" ht="15.75" thickBot="1">
+    <row r="3" spans="1:4" ht="26.25" thickBot="1">
       <c r="A3" s="7">
         <v>2</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="8"/>
+      <c r="B3" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>26</v>
+      </c>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:4" ht="15.75" thickBot="1">
+    <row r="4" spans="1:4" ht="26.25" thickBot="1">
       <c r="A4" s="7">
         <v>3</v>
       </c>
-      <c r="B4" s="6"/>
+      <c r="B4" s="6" t="s">
+        <v>28</v>
+      </c>
       <c r="C4" s="8"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:4" ht="15.75" thickBot="1">
+    <row r="5" spans="1:4" ht="26.25" thickBot="1">
       <c r="A5" s="7">
         <v>4</v>
       </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="8"/>
+      <c r="B5" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="6" spans="1:4" ht="15.75" thickBot="1">
       <c r="A6" s="7">

</xml_diff>

<commit_message>
Nuevo informe testing, actualizacion de CPs
</commit_message>
<xml_diff>
--- a/Producto/Web/Casos de prueba/10.xlsx
+++ b/Producto/Web/Casos de prueba/10.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="6810" yWindow="315" windowWidth="14805" windowHeight="7950" activeTab="2"/>
+    <workbookView xWindow="6810" yWindow="315" windowWidth="14805" windowHeight="7950"/>
   </bookViews>
   <sheets>
     <sheet name="DatosGenerales" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="Pasos" sheetId="2" r:id="rId3"/>
     <sheet name="Control de cambios" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -115,8 +115,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -376,6 +376,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -410,6 +411,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -585,20 +587,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="35.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.5" thickBot="1">
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -606,7 +608,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="16.5" thickBot="1">
+    <row r="2" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -614,7 +616,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="16.5" thickBot="1">
+    <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -622,7 +624,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="32.25" thickBot="1">
+    <row r="4" spans="1:2" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
@@ -630,7 +632,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="16.5" thickBot="1">
+    <row r="5" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
@@ -639,7 +641,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="16.5" thickBot="1">
+    <row r="6" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
@@ -647,7 +649,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="16.5" thickBot="1">
+    <row r="7" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>9</v>
       </c>
@@ -665,20 +667,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="42.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16.5" thickBot="1">
+    <row r="1" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>4</v>
       </c>
@@ -689,7 +691,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="7">
         <v>1</v>
       </c>
@@ -706,21 +708,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="39.140625" customWidth="1"/>
     <col min="3" max="3" width="41.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.5" thickBot="1">
+    <row r="1" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>4</v>
       </c>
@@ -734,7 +736,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" thickBot="1">
+    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7">
         <v>1</v>
       </c>
@@ -744,7 +746,7 @@
       <c r="C2" s="6"/>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:4" ht="26.25" thickBot="1">
+    <row r="3" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
         <v>2</v>
       </c>
@@ -756,7 +758,7 @@
       </c>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:4" ht="26.25" thickBot="1">
+    <row r="4" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
         <v>3</v>
       </c>
@@ -766,7 +768,7 @@
       <c r="C4" s="8"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:4" ht="26.25" thickBot="1">
+    <row r="5" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
         <v>4</v>
       </c>
@@ -777,14 +779,14 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15.75" thickBot="1">
+    <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <v>5</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="8"/>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>6</v>
       </c>
@@ -800,14 +802,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
@@ -815,7 +817,7 @@
     <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16.5" thickBot="1">
+    <row r="1" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>13</v>
       </c>
@@ -832,7 +834,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="38.25">
+    <row r="2" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>17</v>
       </c>

</xml_diff>